<commit_message>
Documentação do Segundo Sprint
</commit_message>
<xml_diff>
--- a/_project/Documentação das Sprints.xlsx
+++ b/_project/Documentação das Sprints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12660"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="20610" windowHeight="11640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto" sheetId="1" r:id="rId1"/>
@@ -15,14 +15,14 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tarefas!$A$11:$D$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Tarefas!$A$11:$D$55</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="112">
   <si>
     <t>Dados do projeto</t>
   </si>
@@ -313,6 +313,84 @@
   </si>
   <si>
     <t>Descrição</t>
+  </si>
+  <si>
+    <t>controller projeto</t>
+  </si>
+  <si>
+    <t>controller historias</t>
+  </si>
+  <si>
+    <t>controller funcionalidade</t>
+  </si>
+  <si>
+    <t>controller cronograma</t>
+  </si>
+  <si>
+    <t>controller sprint</t>
+  </si>
+  <si>
+    <t>route projeto</t>
+  </si>
+  <si>
+    <t>route historias</t>
+  </si>
+  <si>
+    <t>route funcionalidade</t>
+  </si>
+  <si>
+    <t>route cronograma</t>
+  </si>
+  <si>
+    <t>route sprint</t>
+  </si>
+  <si>
+    <t>route product backlog</t>
+  </si>
+  <si>
+    <t>controller product backlog</t>
+  </si>
+  <si>
+    <t>view edit product backlog</t>
+  </si>
+  <si>
+    <t>view remove product backlog</t>
+  </si>
+  <si>
+    <t>view edit projeto</t>
+  </si>
+  <si>
+    <t>view remove projeto</t>
+  </si>
+  <si>
+    <t>view edit historias</t>
+  </si>
+  <si>
+    <t>view remove historias</t>
+  </si>
+  <si>
+    <t>view edit funcionalidade</t>
+  </si>
+  <si>
+    <t>view remove funcionalidade</t>
+  </si>
+  <si>
+    <t>view edit cronograma</t>
+  </si>
+  <si>
+    <t>view remove cronograma</t>
+  </si>
+  <si>
+    <t>view edit sprint</t>
+  </si>
+  <si>
+    <t>view remove sprint</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>elaboração</t>
   </si>
 </sst>
 </file>
@@ -626,28 +704,13 @@
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -696,6 +759,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1047,7 +1125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1059,98 +1137,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1215,175 +1293,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="11" t="str">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="34" t="str">
         <f>[1]Projeto!B2</f>
         <v>Sistema de scrum para alunos do técnico</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="35"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="str">
+      <c r="B4" s="8" t="str">
         <f>[1]Projeto!B3</f>
         <v>Robson</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="11" t="str">
+      <c r="B5" s="34" t="str">
         <f>[1]Projeto!B4</f>
         <v>Robson</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="35"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="2"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="32"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="16" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
-        <v>1</v>
-      </c>
-      <c r="B9" s="23" t="s">
+      <c r="A9" s="17">
+        <v>1</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="20" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="17">
         <v>2</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="20" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="17">
         <v>3</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="20" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+      <c r="A12" s="17">
         <v>4</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="20" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22">
+      <c r="A13" s="17">
         <v>5</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
+      <c r="A14" s="17">
         <v>6</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="17">
         <v>7</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="23" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1400,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="35.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,509 +1493,856 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="str">
+      <c r="B3" s="8" t="str">
         <f>[1]Projeto!$B$2</f>
         <v>Sistema de scrum para alunos do técnico</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="str">
+      <c r="B4" s="8" t="str">
         <f>[1]Projeto!$B$3</f>
         <v>Robson</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="str">
+      <c r="B5" s="8" t="str">
         <f>[1]Projeto!$B$4</f>
         <v>Robson</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="str">
+      <c r="B6" s="8" t="str">
         <f>[1]Projeto!$B$8</f>
         <v>Antonio Augusto</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="29" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
-        <v>1</v>
-      </c>
-      <c r="B12" s="29" t="s">
+      <c r="A12" s="24">
+        <v>1</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="29" t="s">
+      <c r="C12" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
-        <v>1</v>
-      </c>
-      <c r="B13" s="29" t="s">
+      <c r="A13" s="24">
+        <v>1</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="29" t="s">
+      <c r="C13" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="29">
-        <v>1</v>
-      </c>
-      <c r="B14" s="29" t="s">
+      <c r="A14" s="24">
+        <v>1</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="29" t="s">
+      <c r="C14" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="24" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
-        <v>1</v>
-      </c>
-      <c r="B15" s="29" t="s">
+      <c r="A15" s="24">
+        <v>1</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" s="29" t="s">
+      <c r="C15" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
-        <v>1</v>
-      </c>
-      <c r="B16" s="29" t="s">
+      <c r="A16" s="24">
+        <v>1</v>
+      </c>
+      <c r="B16" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="29" t="s">
+      <c r="C16" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="24" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29">
-        <v>1</v>
-      </c>
-      <c r="B17" s="29" t="s">
+      <c r="A17" s="24">
+        <v>1</v>
+      </c>
+      <c r="B17" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="29" t="s">
+      <c r="C17" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="24" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
-        <v>1</v>
-      </c>
-      <c r="B18" s="29" t="s">
+      <c r="A18" s="24">
+        <v>1</v>
+      </c>
+      <c r="B18" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="29" t="s">
+      <c r="C18" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="24" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
-        <v>1</v>
-      </c>
-      <c r="B19" s="29" t="s">
+      <c r="A19" s="24">
+        <v>1</v>
+      </c>
+      <c r="B19" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D19" s="29" t="s">
+      <c r="C19" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="24" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
-        <v>1</v>
-      </c>
-      <c r="B20" s="29" t="s">
+      <c r="A20" s="24">
+        <v>1</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="29" t="s">
+      <c r="C20" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
-        <v>1</v>
-      </c>
-      <c r="B21" s="29" t="s">
+      <c r="A21" s="24">
+        <v>1</v>
+      </c>
+      <c r="B21" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="29" t="s">
+      <c r="C21" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="24" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
-        <v>1</v>
-      </c>
-      <c r="B22" s="29" t="s">
+      <c r="A22" s="24">
+        <v>1</v>
+      </c>
+      <c r="B22" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="29" t="s">
+      <c r="C22" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="29">
-        <v>1</v>
-      </c>
-      <c r="B23" s="29" t="s">
+      <c r="A23" s="24">
+        <v>1</v>
+      </c>
+      <c r="B23" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="29" t="s">
+      <c r="C23" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="24" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="29">
-        <v>1</v>
-      </c>
-      <c r="B24" s="29" t="s">
+      <c r="A24" s="24">
+        <v>1</v>
+      </c>
+      <c r="B24" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="30" t="s">
+      <c r="C24" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="25" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
-        <v>1</v>
-      </c>
-      <c r="B25" s="29" t="s">
+      <c r="A25" s="24">
+        <v>1</v>
+      </c>
+      <c r="B25" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="30" t="s">
+      <c r="C25" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="25" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="29">
-        <v>1</v>
-      </c>
-      <c r="B26" s="29" t="s">
+      <c r="A26" s="24">
+        <v>1</v>
+      </c>
+      <c r="B26" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="30" t="s">
+      <c r="C26" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="25" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="29">
-        <v>1</v>
-      </c>
-      <c r="B27" s="29" t="s">
+      <c r="A27" s="24">
+        <v>1</v>
+      </c>
+      <c r="B27" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="30" t="s">
+      <c r="C27" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="25" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="29">
-        <v>1</v>
-      </c>
-      <c r="B28" s="30" t="s">
+      <c r="A28" s="24">
+        <v>1</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="24">
+        <v>1</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="24">
+        <v>1</v>
+      </c>
+      <c r="B30" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="30" t="s">
+      <c r="C30" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="25" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="29">
-        <v>1</v>
-      </c>
-      <c r="B29" s="29" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="24">
+        <v>1</v>
+      </c>
+      <c r="B31" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="30" t="s">
+      <c r="C31" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="29">
-        <v>1</v>
-      </c>
-      <c r="B30" s="29" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="24">
+        <v>1</v>
+      </c>
+      <c r="B32" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="30" t="s">
+      <c r="C32" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="29">
-        <v>1</v>
-      </c>
-      <c r="B31" s="29" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="24">
+        <v>1</v>
+      </c>
+      <c r="B33" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="30" t="s">
+      <c r="C33" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="29">
-        <v>1</v>
-      </c>
-      <c r="B32" s="29" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="24">
+        <v>1</v>
+      </c>
+      <c r="B34" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D32" s="30" t="s">
+      <c r="C34" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="29">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="24">
         <v>2</v>
       </c>
-      <c r="B33" s="29" t="s">
+      <c r="B35" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C35" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="24">
+        <v>2</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="24">
+        <v>2</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="24">
+        <v>2</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="24">
+        <v>2</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="24">
+        <v>2</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="29" t="s">
+      <c r="D40" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="24">
+        <v>2</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="24">
+        <v>2</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="24">
+        <v>2</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D43" s="25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="29">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="24">
         <v>2</v>
       </c>
-      <c r="B34" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="29" t="s">
+      <c r="B44" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="24">
+        <v>2</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D34" s="29" t="s">
+      <c r="D45" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="24">
+        <v>2</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="24">
+        <v>2</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="24">
+        <v>2</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="29">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="24">
         <v>2</v>
       </c>
-      <c r="B35" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="29" t="s">
+      <c r="B49" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="24">
+        <v>2</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="29" t="s">
+      <c r="D50" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="24">
+        <v>2</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D51" s="24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="24">
+        <v>2</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="24">
+        <v>2</v>
+      </c>
+      <c r="B53" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53" s="25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="29">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="24">
         <v>2</v>
       </c>
-      <c r="B36" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C36" s="29" t="s">
+      <c r="B54" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C54" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="24">
+        <v>2</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="25">
+        <v>3</v>
+      </c>
+      <c r="B56" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D56" s="25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="29">
-        <v>2</v>
-      </c>
-      <c r="B37" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="29" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="25">
+        <v>3</v>
+      </c>
+      <c r="B57" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C57" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D57" s="25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="29">
-        <v>2</v>
-      </c>
-      <c r="B38" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" s="29" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="25">
+        <v>3</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D58" s="25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="29">
-        <v>2</v>
-      </c>
-      <c r="B39" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="29" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="25">
+        <v>3</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="D59" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="25">
+        <v>3</v>
+      </c>
+      <c r="B60" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D60" s="25" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="29">
-        <v>2</v>
-      </c>
-      <c r="B40" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" s="29" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="25">
+        <v>3</v>
+      </c>
+      <c r="B61" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C61" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D61" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="25">
+        <v>3</v>
+      </c>
+      <c r="B62" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" s="25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="29">
-        <v>2</v>
-      </c>
-      <c r="B41" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="29" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="25">
+        <v>3</v>
+      </c>
+      <c r="B63" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D63" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="25">
+        <v>3</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C64" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" s="25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="5"/>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="25">
+        <v>3</v>
+      </c>
+      <c r="B65" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C65" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="25">
+        <v>3</v>
+      </c>
+      <c r="B66" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D66" s="25" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A11:D41">
-    <sortState ref="A12:D41">
-      <sortCondition ref="A11:A41"/>
+  <autoFilter ref="A11:D55">
+    <sortState ref="A12:D55">
+      <sortCondition ref="A11:A43"/>
     </sortState>
   </autoFilter>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Set charser no mysqli e ordenando titulos no header
</commit_message>
<xml_diff>
--- a/_project/Documentação das Sprints.xlsx
+++ b/_project/Documentação das Sprints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="20610" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="20610" windowHeight="11640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="115">
   <si>
     <t>Dados do projeto</t>
   </si>
@@ -395,6 +395,12 @@
   </si>
   <si>
     <t>Notas</t>
+  </si>
+  <si>
+    <t>Lucas atrasou a entrega da Sprint</t>
+  </si>
+  <si>
+    <t>Marina teve mais trabalho que os demais, Camilli ajudou Marina</t>
   </si>
 </sst>
 </file>
@@ -778,6 +784,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -786,9 +795,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1297,24 +1303,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="36" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1334,7 +1340,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1354,7 +1360,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1368,14 +1374,37 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="H4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1405,8 +1434,8 @@
       <c r="A1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1419,12 +1448,12 @@
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="34" t="str">
+      <c r="B3" s="35" t="str">
         <f>[1]Projeto!B2</f>
         <v>Sistema de scrum para alunos do técnico</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -1441,12 +1470,12 @@
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="34" t="str">
+      <c r="B5" s="35" t="str">
         <f>[1]Projeto!B4</f>
         <v>Robson</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
@@ -1458,8 +1487,8 @@
       <c r="A7" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="32"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1589,7 +1618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
@@ -1660,9 +1689,9 @@
     </row>
     <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">

</xml_diff>